<commit_message>
Added a few bugs for withdrawal, session, balance
</commit_message>
<xml_diff>
--- a/Bug Reports/Scripted Defect Report.xlsx
+++ b/Bug Reports/Scripted Defect Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gladius/Documents/SENG 637/Assignment 1/a1-ExGranite/Bug Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saadz-khan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0C0FEC-DC44-F14F-8050-ACAB400BC580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EE9D17-5A58-7149-8D14-F3AB14C0EEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="960" windowWidth="33420" windowHeight="21140" xr2:uid="{A07C5CE1-8239-7940-856B-018EAA5653E2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{A07C5CE1-8239-7940-856B-018EAA5653E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -897,7 +897,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>